<commit_message>
fix demand data error
</commit_message>
<xml_diff>
--- a/data/capacity_factor_and_demand_calcs.xlsx
+++ b/data/capacity_factor_and_demand_calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z5076823\version_control\sola5050\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61679E9-BF45-437F-B5CD-BE017335B01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF053C01-DB11-4764-91D9-C3AF4E2BC551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_OpenNEM_data" sheetId="1" r:id="rId1"/>
@@ -23468,7 +23468,7 @@
   <dimension ref="A1:G338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L321" sqref="L321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23527,7 +23527,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
+        <f>SUM(raw_OpenNEM_data!$D2:$E2,raw_OpenNEM_data!$G2:$L2)</f>
         <v>7641.119999999999</v>
       </c>
     </row>
@@ -23556,8 +23556,8 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D3:$E3,raw_OpenNEM_data!$G3:$L3)</f>
+        <v>7706.96</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -23585,8 +23585,8 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D4:$E4,raw_OpenNEM_data!$G4:$L4)</f>
+        <v>7816.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -23614,8 +23614,8 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D5:$E5,raw_OpenNEM_data!$G5:$L5)</f>
+        <v>7729.91</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -23643,8 +23643,8 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D6:$E6,raw_OpenNEM_data!$G6:$L6)</f>
+        <v>7733.6999999999989</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -23672,8 +23672,8 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D7:$E7,raw_OpenNEM_data!$G7:$L7)</f>
+        <v>7652.16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -23701,8 +23701,8 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D8:$E8,raw_OpenNEM_data!$G8:$L8)</f>
+        <v>7527.5899999999992</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -23730,8 +23730,8 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D9:$E9,raw_OpenNEM_data!$G9:$L9)</f>
+        <v>7364.03</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -23759,8 +23759,8 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D10:$E10,raw_OpenNEM_data!$G10:$L10)</f>
+        <v>7221.71</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -23788,8 +23788,8 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D11:$E11,raw_OpenNEM_data!$G11:$L11)</f>
+        <v>6993.65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -23817,8 +23817,8 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D12:$E12,raw_OpenNEM_data!$G12:$L12)</f>
+        <v>6949.6699999999992</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -23846,8 +23846,8 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D13:$E13,raw_OpenNEM_data!$G13:$L13)</f>
+        <v>6757.93</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -23875,8 +23875,8 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D14:$E14,raw_OpenNEM_data!$G14:$L14)</f>
+        <v>6559.12</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -23904,8 +23904,8 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D15:$E15,raw_OpenNEM_data!$G15:$L15)</f>
+        <v>6526.27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -23933,8 +23933,8 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D16:$E16,raw_OpenNEM_data!$G16:$L16)</f>
+        <v>6287.87</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -23962,8 +23962,8 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D17:$E17,raw_OpenNEM_data!$G17:$L17)</f>
+        <v>6081.76</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -23991,8 +23991,8 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D18:$E18,raw_OpenNEM_data!$G18:$L18)</f>
+        <v>5873.9800000000005</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -24020,8 +24020,8 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D19:$E19,raw_OpenNEM_data!$G19:$L19)</f>
+        <v>5700.9</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -24049,8 +24049,8 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D20:$E20,raw_OpenNEM_data!$G20:$L20)</f>
+        <v>5560.9900000000007</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -24078,8 +24078,8 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D21:$E21,raw_OpenNEM_data!$G21:$L21)</f>
+        <v>5570.4800000000005</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -24107,8 +24107,8 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D22:$E22,raw_OpenNEM_data!$G22:$L22)</f>
+        <v>5524.47</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -24136,8 +24136,8 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D23:$E23,raw_OpenNEM_data!$G23:$L23)</f>
+        <v>5542.1500000000005</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -24165,8 +24165,8 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D24:$E24,raw_OpenNEM_data!$G24:$L24)</f>
+        <v>5596.28</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -24194,8 +24194,8 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D25:$E25,raw_OpenNEM_data!$G25:$L25)</f>
+        <v>5642.57</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -24223,8 +24223,8 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D26:$E26,raw_OpenNEM_data!$G26:$L26)</f>
+        <v>5784.42</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -24252,8 +24252,8 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D27:$E27,raw_OpenNEM_data!$G27:$L27)</f>
+        <v>5995.9600000000009</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -24281,8 +24281,8 @@
         <v>1</v>
       </c>
       <c r="G28">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D28:$E28,raw_OpenNEM_data!$G28:$L28)</f>
+        <v>6304.4300000000012</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -24310,8 +24310,8 @@
         <v>1</v>
       </c>
       <c r="G29">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D29:$E29,raw_OpenNEM_data!$G29:$L29)</f>
+        <v>6682.0400000000009</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -24339,8 +24339,8 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D30:$E30,raw_OpenNEM_data!$G30:$L30)</f>
+        <v>7165.7199999999993</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -24368,8 +24368,8 @@
         <v>1</v>
       </c>
       <c r="G31">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D31:$E31,raw_OpenNEM_data!$G31:$L31)</f>
+        <v>7434.2899999999991</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -24397,8 +24397,8 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D32:$E32,raw_OpenNEM_data!$G32:$L32)</f>
+        <v>7821</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -24426,8 +24426,8 @@
         <v>1</v>
       </c>
       <c r="G33">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D33:$E33,raw_OpenNEM_data!$G33:$L33)</f>
+        <v>7949.38</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -24455,8 +24455,8 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D34:$E34,raw_OpenNEM_data!$G34:$L34)</f>
+        <v>8075.4500000000007</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -24484,8 +24484,8 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D35:$E35,raw_OpenNEM_data!$G35:$L35)</f>
+        <v>8179.02</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -24513,8 +24513,8 @@
         <v>1</v>
       </c>
       <c r="G36">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D36:$E36,raw_OpenNEM_data!$G36:$L36)</f>
+        <v>8442.15</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -24542,8 +24542,8 @@
         <v>1</v>
       </c>
       <c r="G37">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D37:$E37,raw_OpenNEM_data!$G37:$L37)</f>
+        <v>8445.9500000000007</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -24571,8 +24571,8 @@
         <v>1</v>
       </c>
       <c r="G38">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D38:$E38,raw_OpenNEM_data!$G38:$L38)</f>
+        <v>8476.0700000000015</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -24600,8 +24600,8 @@
         <v>1</v>
       </c>
       <c r="G39">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D39:$E39,raw_OpenNEM_data!$G39:$L39)</f>
+        <v>8492.91</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -24629,8 +24629,8 @@
         <v>1</v>
       </c>
       <c r="G40">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D40:$E40,raw_OpenNEM_data!$G40:$L40)</f>
+        <v>8476.61</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -24658,8 +24658,8 @@
         <v>1</v>
       </c>
       <c r="G41">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D41:$E41,raw_OpenNEM_data!$G41:$L41)</f>
+        <v>8569.02</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -24687,8 +24687,8 @@
         <v>1</v>
       </c>
       <c r="G42">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D42:$E42,raw_OpenNEM_data!$G42:$L42)</f>
+        <v>8614.64</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -24716,8 +24716,8 @@
         <v>1</v>
       </c>
       <c r="G43">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D43:$E43,raw_OpenNEM_data!$G43:$L43)</f>
+        <v>8758.18</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -24745,8 +24745,8 @@
         <v>1</v>
       </c>
       <c r="G44">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D44:$E44,raw_OpenNEM_data!$G44:$L44)</f>
+        <v>8839.9</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -24774,8 +24774,8 @@
         <v>1</v>
       </c>
       <c r="G45">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D45:$E45,raw_OpenNEM_data!$G45:$L45)</f>
+        <v>8853.0999999999985</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -24803,8 +24803,8 @@
         <v>1</v>
       </c>
       <c r="G46">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D46:$E46,raw_OpenNEM_data!$G46:$L46)</f>
+        <v>8934.68</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -24832,8 +24832,8 @@
         <v>1</v>
       </c>
       <c r="G47">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D47:$E47,raw_OpenNEM_data!$G47:$L47)</f>
+        <v>9003</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -24861,8 +24861,8 @@
         <v>1</v>
       </c>
       <c r="G48">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D48:$E48,raw_OpenNEM_data!$G48:$L48)</f>
+        <v>8961.1299999999992</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -24890,8 +24890,8 @@
         <v>1</v>
       </c>
       <c r="G49">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D49:$E49,raw_OpenNEM_data!$G49:$L49)</f>
+        <v>9110.83</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -24919,8 +24919,8 @@
         <v>1</v>
       </c>
       <c r="G50">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D50:$E50,raw_OpenNEM_data!$G50:$L50)</f>
+        <v>8917.44</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -24948,8 +24948,8 @@
         <v>1</v>
       </c>
       <c r="G51">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D51:$E51,raw_OpenNEM_data!$G51:$L51)</f>
+        <v>8775.010000000002</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -24977,8 +24977,8 @@
         <v>1</v>
       </c>
       <c r="G52">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D52:$E52,raw_OpenNEM_data!$G52:$L52)</f>
+        <v>8584.14</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -25006,8 +25006,8 @@
         <v>1</v>
       </c>
       <c r="G53">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D53:$E53,raw_OpenNEM_data!$G53:$L53)</f>
+        <v>8461.840000000002</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -25035,8 +25035,8 @@
         <v>1</v>
       </c>
       <c r="G54">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D54:$E54,raw_OpenNEM_data!$G54:$L54)</f>
+        <v>8420.8100000000013</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -25064,8 +25064,8 @@
         <v>1</v>
       </c>
       <c r="G55">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D55:$E55,raw_OpenNEM_data!$G55:$L55)</f>
+        <v>8287.4500000000007</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -25093,8 +25093,8 @@
         <v>1</v>
       </c>
       <c r="G56">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D56:$E56,raw_OpenNEM_data!$G56:$L56)</f>
+        <v>8148.41</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -25122,8 +25122,8 @@
         <v>1</v>
       </c>
       <c r="G57">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D57:$E57,raw_OpenNEM_data!$G57:$L57)</f>
+        <v>7908.9400000000005</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -25151,8 +25151,8 @@
         <v>1</v>
       </c>
       <c r="G58">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D58:$E58,raw_OpenNEM_data!$G58:$L58)</f>
+        <v>7776.5999999999995</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -25180,8 +25180,8 @@
         <v>1</v>
       </c>
       <c r="G59">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D59:$E59,raw_OpenNEM_data!$G59:$L59)</f>
+        <v>7637.4199999999992</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -25209,8 +25209,8 @@
         <v>1</v>
       </c>
       <c r="G60">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D60:$E60,raw_OpenNEM_data!$G60:$L60)</f>
+        <v>7439.119999999999</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -25238,8 +25238,8 @@
         <v>1</v>
       </c>
       <c r="G61">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D61:$E61,raw_OpenNEM_data!$G61:$L61)</f>
+        <v>7179.57</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -25267,8 +25267,8 @@
         <v>1</v>
       </c>
       <c r="G62">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D62:$E62,raw_OpenNEM_data!$G62:$L62)</f>
+        <v>6997.01</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -25296,8 +25296,8 @@
         <v>1</v>
       </c>
       <c r="G63">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D63:$E63,raw_OpenNEM_data!$G63:$L63)</f>
+        <v>6844.0499999999993</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -25325,8 +25325,8 @@
         <v>1</v>
       </c>
       <c r="G64">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D64:$E64,raw_OpenNEM_data!$G64:$L64)</f>
+        <v>6596.1900000000005</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -25354,8 +25354,8 @@
         <v>1</v>
       </c>
       <c r="G65">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D65:$E65,raw_OpenNEM_data!$G65:$L65)</f>
+        <v>6419.8100000000013</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -25383,8 +25383,8 @@
         <v>1</v>
       </c>
       <c r="G66">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D66:$E66,raw_OpenNEM_data!$G66:$L66)</f>
+        <v>6187.4999999999991</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -25412,8 +25412,8 @@
         <v>1</v>
       </c>
       <c r="G67">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D67:$E67,raw_OpenNEM_data!$G67:$L67)</f>
+        <v>6022.35</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -25441,8 +25441,8 @@
         <v>1</v>
       </c>
       <c r="G68">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D68:$E68,raw_OpenNEM_data!$G68:$L68)</f>
+        <v>5963.670000000001</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -25470,8 +25470,8 @@
         <v>1</v>
       </c>
       <c r="G69">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D69:$E69,raw_OpenNEM_data!$G69:$L69)</f>
+        <v>5892.86</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -25499,8 +25499,8 @@
         <v>1</v>
       </c>
       <c r="G70">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D70:$E70,raw_OpenNEM_data!$G70:$L70)</f>
+        <v>5896.37</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -25528,8 +25528,8 @@
         <v>1</v>
       </c>
       <c r="G71">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D71:$E71,raw_OpenNEM_data!$G71:$L71)</f>
+        <v>5900.55</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -25557,8 +25557,8 @@
         <v>1</v>
       </c>
       <c r="G72">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D72:$E72,raw_OpenNEM_data!$G72:$L72)</f>
+        <v>5966.5000000000009</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -25586,8 +25586,8 @@
         <v>1</v>
       </c>
       <c r="G73">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D73:$E73,raw_OpenNEM_data!$G73:$L73)</f>
+        <v>6046.92</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -25615,8 +25615,8 @@
         <v>1</v>
       </c>
       <c r="G74">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D74:$E74,raw_OpenNEM_data!$G74:$L74)</f>
+        <v>6225.61</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -25644,8 +25644,8 @@
         <v>1</v>
       </c>
       <c r="G75">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D75:$E75,raw_OpenNEM_data!$G75:$L75)</f>
+        <v>6464.48</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -25673,8 +25673,8 @@
         <v>1</v>
       </c>
       <c r="G76">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D76:$E76,raw_OpenNEM_data!$G76:$L76)</f>
+        <v>6651.1900000000005</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -25702,8 +25702,8 @@
         <v>1</v>
       </c>
       <c r="G77">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D77:$E77,raw_OpenNEM_data!$G77:$L77)</f>
+        <v>6916.01</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -25731,8 +25731,8 @@
         <v>1</v>
       </c>
       <c r="G78">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D78:$E78,raw_OpenNEM_data!$G78:$L78)</f>
+        <v>7249.3099999999995</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -25760,8 +25760,8 @@
         <v>1</v>
       </c>
       <c r="G79">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D79:$E79,raw_OpenNEM_data!$G79:$L79)</f>
+        <v>7609.29</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -25789,8 +25789,8 @@
         <v>1</v>
       </c>
       <c r="G80">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D80:$E80,raw_OpenNEM_data!$G80:$L80)</f>
+        <v>7885.3399999999992</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -25818,8 +25818,8 @@
         <v>1</v>
       </c>
       <c r="G81">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D81:$E81,raw_OpenNEM_data!$G81:$L81)</f>
+        <v>8294.77</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -25847,8 +25847,8 @@
         <v>1</v>
       </c>
       <c r="G82">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D82:$E82,raw_OpenNEM_data!$G82:$L82)</f>
+        <v>8489.9500000000007</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -25876,8 +25876,8 @@
         <v>1</v>
       </c>
       <c r="G83">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D83:$E83,raw_OpenNEM_data!$G83:$L83)</f>
+        <v>8676.27</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -25905,8 +25905,8 @@
         <v>1</v>
       </c>
       <c r="G84">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D84:$E84,raw_OpenNEM_data!$G84:$L84)</f>
+        <v>8793.24</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -25934,8 +25934,8 @@
         <v>1</v>
       </c>
       <c r="G85">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D85:$E85,raw_OpenNEM_data!$G85:$L85)</f>
+        <v>8824.4699999999993</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -25963,8 +25963,8 @@
         <v>1</v>
       </c>
       <c r="G86">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D86:$E86,raw_OpenNEM_data!$G86:$L86)</f>
+        <v>8963.85</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -25992,8 +25992,8 @@
         <v>1</v>
       </c>
       <c r="G87">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D87:$E87,raw_OpenNEM_data!$G87:$L87)</f>
+        <v>8852.82</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -26021,8 +26021,8 @@
         <v>1</v>
       </c>
       <c r="G88">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D88:$E88,raw_OpenNEM_data!$G88:$L88)</f>
+        <v>8849.2899999999991</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -26050,8 +26050,8 @@
         <v>1</v>
       </c>
       <c r="G89">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D89:$E89,raw_OpenNEM_data!$G89:$L89)</f>
+        <v>8784.74</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -26079,8 +26079,8 @@
         <v>1</v>
       </c>
       <c r="G90">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D90:$E90,raw_OpenNEM_data!$G90:$L90)</f>
+        <v>8594.2200000000012</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -26108,8 +26108,8 @@
         <v>1</v>
       </c>
       <c r="G91">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D91:$E91,raw_OpenNEM_data!$G91:$L91)</f>
+        <v>8422.2799999999988</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -26137,8 +26137,8 @@
         <v>1</v>
       </c>
       <c r="G92">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D92:$E92,raw_OpenNEM_data!$G92:$L92)</f>
+        <v>8294.82</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -26166,8 +26166,8 @@
         <v>1</v>
       </c>
       <c r="G93">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D93:$E93,raw_OpenNEM_data!$G93:$L93)</f>
+        <v>8072.6900000000005</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -26195,8 +26195,8 @@
         <v>1</v>
       </c>
       <c r="G94">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D94:$E94,raw_OpenNEM_data!$G94:$L94)</f>
+        <v>8046.99</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -26224,8 +26224,8 @@
         <v>1</v>
       </c>
       <c r="G95">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D95:$E95,raw_OpenNEM_data!$G95:$L95)</f>
+        <v>8110.57</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -26253,8 +26253,8 @@
         <v>1</v>
       </c>
       <c r="G96">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D96:$E96,raw_OpenNEM_data!$G96:$L96)</f>
+        <v>8062.5199999999986</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -26282,8 +26282,8 @@
         <v>1</v>
       </c>
       <c r="G97">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D97:$E97,raw_OpenNEM_data!$G97:$L97)</f>
+        <v>8191.09</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -26311,8 +26311,8 @@
         <v>1</v>
       </c>
       <c r="G98">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D98:$E98,raw_OpenNEM_data!$G98:$L98)</f>
+        <v>8068.5900000000011</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -26340,8 +26340,8 @@
         <v>1</v>
       </c>
       <c r="G99">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D99:$E99,raw_OpenNEM_data!$G99:$L99)</f>
+        <v>7886.7400000000007</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -26369,8 +26369,8 @@
         <v>1</v>
       </c>
       <c r="G100">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D100:$E100,raw_OpenNEM_data!$G100:$L100)</f>
+        <v>7650.1900000000005</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -26398,8 +26398,8 @@
         <v>1</v>
       </c>
       <c r="G101">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D101:$E101,raw_OpenNEM_data!$G101:$L101)</f>
+        <v>7489.8</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -26427,8 +26427,8 @@
         <v>1</v>
       </c>
       <c r="G102">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D102:$E102,raw_OpenNEM_data!$G102:$L102)</f>
+        <v>7458.4500000000016</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -26456,8 +26456,8 @@
         <v>1</v>
       </c>
       <c r="G103">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D103:$E103,raw_OpenNEM_data!$G103:$L103)</f>
+        <v>7344.7399999999989</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -26485,8 +26485,8 @@
         <v>1</v>
       </c>
       <c r="G104">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D104:$E104,raw_OpenNEM_data!$G104:$L104)</f>
+        <v>7214.79</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -26514,8 +26514,8 @@
         <v>1</v>
       </c>
       <c r="G105">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D105:$E105,raw_OpenNEM_data!$G105:$L105)</f>
+        <v>7127.4900000000007</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -26543,8 +26543,8 @@
         <v>1</v>
       </c>
       <c r="G106">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D106:$E106,raw_OpenNEM_data!$G106:$L106)</f>
+        <v>7114.83</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -26572,8 +26572,8 @@
         <v>1</v>
       </c>
       <c r="G107">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D107:$E107,raw_OpenNEM_data!$G107:$L107)</f>
+        <v>7038.47</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -26601,8 +26601,8 @@
         <v>1</v>
       </c>
       <c r="G108">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D108:$E108,raw_OpenNEM_data!$G108:$L108)</f>
+        <v>6988.9299999999994</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -26630,8 +26630,8 @@
         <v>1</v>
       </c>
       <c r="G109">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D109:$E109,raw_OpenNEM_data!$G109:$L109)</f>
+        <v>6892.6100000000006</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -26659,8 +26659,8 @@
         <v>1</v>
       </c>
       <c r="G110">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D110:$E110,raw_OpenNEM_data!$G110:$L110)</f>
+        <v>6871.67</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -26688,8 +26688,8 @@
         <v>1</v>
       </c>
       <c r="G111">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D111:$E111,raw_OpenNEM_data!$G111:$L111)</f>
+        <v>6726.15</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -26717,8 +26717,8 @@
         <v>1</v>
       </c>
       <c r="G112">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D112:$E112,raw_OpenNEM_data!$G112:$L112)</f>
+        <v>6528.22</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
@@ -26746,8 +26746,8 @@
         <v>1</v>
       </c>
       <c r="G113">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D113:$E113,raw_OpenNEM_data!$G113:$L113)</f>
+        <v>6325.1299999999992</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -26775,8 +26775,8 @@
         <v>1</v>
       </c>
       <c r="G114">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D114:$E114,raw_OpenNEM_data!$G114:$L114)</f>
+        <v>6060.34</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -26804,8 +26804,8 @@
         <v>1</v>
       </c>
       <c r="G115">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D115:$E115,raw_OpenNEM_data!$G115:$L115)</f>
+        <v>5872.4900000000007</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
@@ -26833,8 +26833,8 @@
         <v>1</v>
       </c>
       <c r="G116">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D116:$E116,raw_OpenNEM_data!$G116:$L116)</f>
+        <v>5791.2599999999993</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -26862,8 +26862,8 @@
         <v>1</v>
       </c>
       <c r="G117">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D117:$E117,raw_OpenNEM_data!$G117:$L117)</f>
+        <v>5699.3199999999988</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -26891,8 +26891,8 @@
         <v>1</v>
       </c>
       <c r="G118">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D118:$E118,raw_OpenNEM_data!$G118:$L118)</f>
+        <v>5676.79</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -26920,8 +26920,8 @@
         <v>1</v>
       </c>
       <c r="G119">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D119:$E119,raw_OpenNEM_data!$G119:$L119)</f>
+        <v>5689.1500000000005</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -26949,8 +26949,8 @@
         <v>1</v>
       </c>
       <c r="G120">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D120:$E120,raw_OpenNEM_data!$G120:$L120)</f>
+        <v>5851.7400000000016</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -26978,8 +26978,8 @@
         <v>1</v>
       </c>
       <c r="G121">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D121:$E121,raw_OpenNEM_data!$G121:$L121)</f>
+        <v>5958.49</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -27007,8 +27007,8 @@
         <v>1</v>
       </c>
       <c r="G122">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D122:$E122,raw_OpenNEM_data!$G122:$L122)</f>
+        <v>6220.3600000000006</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -27036,8 +27036,8 @@
         <v>1</v>
       </c>
       <c r="G123">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D123:$E123,raw_OpenNEM_data!$G123:$L123)</f>
+        <v>6500.67</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -27065,8 +27065,8 @@
         <v>1</v>
       </c>
       <c r="G124">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D124:$E124,raw_OpenNEM_data!$G124:$L124)</f>
+        <v>6795.4699999999993</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -27094,8 +27094,8 @@
         <v>1</v>
       </c>
       <c r="G125">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D125:$E125,raw_OpenNEM_data!$G125:$L125)</f>
+        <v>7023.46</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
@@ -27123,8 +27123,8 @@
         <v>1</v>
       </c>
       <c r="G126">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D126:$E126,raw_OpenNEM_data!$G126:$L126)</f>
+        <v>7437.4800000000005</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
@@ -27152,8 +27152,8 @@
         <v>1</v>
       </c>
       <c r="G127">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D127:$E127,raw_OpenNEM_data!$G127:$L127)</f>
+        <v>7684.58</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
@@ -27181,8 +27181,8 @@
         <v>1</v>
       </c>
       <c r="G128">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D128:$E128,raw_OpenNEM_data!$G128:$L128)</f>
+        <v>7878.46</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -27210,8 +27210,8 @@
         <v>1</v>
       </c>
       <c r="G129">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D129:$E129,raw_OpenNEM_data!$G129:$L129)</f>
+        <v>7948.3000000000011</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
@@ -27239,8 +27239,8 @@
         <v>1</v>
       </c>
       <c r="G130">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D130:$E130,raw_OpenNEM_data!$G130:$L130)</f>
+        <v>7991.43</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -27268,8 +27268,8 @@
         <v>1</v>
       </c>
       <c r="G131">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D131:$E131,raw_OpenNEM_data!$G131:$L131)</f>
+        <v>8047.99</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -27297,8 +27297,8 @@
         <v>1</v>
       </c>
       <c r="G132">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D132:$E132,raw_OpenNEM_data!$G132:$L132)</f>
+        <v>8169.48</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -27326,8 +27326,8 @@
         <v>1</v>
       </c>
       <c r="G133">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D133:$E133,raw_OpenNEM_data!$G133:$L133)</f>
+        <v>8096.4300000000012</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -27355,8 +27355,8 @@
         <v>1</v>
       </c>
       <c r="G134">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D134:$E134,raw_OpenNEM_data!$G134:$L134)</f>
+        <v>8001.6900000000005</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
@@ -27384,8 +27384,8 @@
         <v>1</v>
       </c>
       <c r="G135">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D135:$E135,raw_OpenNEM_data!$G135:$L135)</f>
+        <v>8069.08</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
@@ -27413,8 +27413,8 @@
         <v>1</v>
       </c>
       <c r="G136">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D136:$E136,raw_OpenNEM_data!$G136:$L136)</f>
+        <v>8085.8600000000006</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -27442,8 +27442,8 @@
         <v>1</v>
       </c>
       <c r="G137">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D137:$E137,raw_OpenNEM_data!$G137:$L137)</f>
+        <v>8081.93</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -27471,8 +27471,8 @@
         <v>1</v>
       </c>
       <c r="G138">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D138:$E138,raw_OpenNEM_data!$G138:$L138)</f>
+        <v>8010.82</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -27500,8 +27500,8 @@
         <v>1</v>
       </c>
       <c r="G139">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D139:$E139,raw_OpenNEM_data!$G139:$L139)</f>
+        <v>7828.8799999999992</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
@@ -27529,8 +27529,8 @@
         <v>1</v>
       </c>
       <c r="G140">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D140:$E140,raw_OpenNEM_data!$G140:$L140)</f>
+        <v>7900.4499999999989</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -27558,8 +27558,8 @@
         <v>1</v>
       </c>
       <c r="G141">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D141:$E141,raw_OpenNEM_data!$G141:$L141)</f>
+        <v>7893.39</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -27587,8 +27587,8 @@
         <v>1</v>
       </c>
       <c r="G142">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D142:$E142,raw_OpenNEM_data!$G142:$L142)</f>
+        <v>7944.1400000000012</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -27616,8 +27616,8 @@
         <v>1</v>
       </c>
       <c r="G143">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D143:$E143,raw_OpenNEM_data!$G143:$L143)</f>
+        <v>7942.0899999999983</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -27645,8 +27645,8 @@
         <v>1</v>
       </c>
       <c r="G144">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D144:$E144,raw_OpenNEM_data!$G144:$L144)</f>
+        <v>7953.51</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -27674,8 +27674,8 @@
         <v>1</v>
       </c>
       <c r="G145">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D145:$E145,raw_OpenNEM_data!$G145:$L145)</f>
+        <v>8022.56</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -27703,8 +27703,8 @@
         <v>1</v>
       </c>
       <c r="G146">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D146:$E146,raw_OpenNEM_data!$G146:$L146)</f>
+        <v>7990.8799999999992</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -27732,8 +27732,8 @@
         <v>1</v>
       </c>
       <c r="G147">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D147:$E147,raw_OpenNEM_data!$G147:$L147)</f>
+        <v>7864.2199999999993</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -27761,8 +27761,8 @@
         <v>1</v>
       </c>
       <c r="G148">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D148:$E148,raw_OpenNEM_data!$G148:$L148)</f>
+        <v>7627.69</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -27790,8 +27790,8 @@
         <v>1</v>
       </c>
       <c r="G149">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D149:$E149,raw_OpenNEM_data!$G149:$L149)</f>
+        <v>7551.3200000000006</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -27819,8 +27819,8 @@
         <v>1</v>
       </c>
       <c r="G150">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D150:$E150,raw_OpenNEM_data!$G150:$L150)</f>
+        <v>7591.41</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -27848,8 +27848,8 @@
         <v>1</v>
       </c>
       <c r="G151">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D151:$E151,raw_OpenNEM_data!$G151:$L151)</f>
+        <v>7602.6</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -27877,8 +27877,8 @@
         <v>1</v>
       </c>
       <c r="G152">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D152:$E152,raw_OpenNEM_data!$G152:$L152)</f>
+        <v>7689.0999999999995</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -27906,8 +27906,8 @@
         <v>1</v>
       </c>
       <c r="G153">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D153:$E153,raw_OpenNEM_data!$G153:$L153)</f>
+        <v>7580.6800000000012</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -27935,8 +27935,8 @@
         <v>1</v>
       </c>
       <c r="G154">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D154:$E154,raw_OpenNEM_data!$G154:$L154)</f>
+        <v>7586.93</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -27964,8 +27964,8 @@
         <v>1</v>
       </c>
       <c r="G155">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D155:$E155,raw_OpenNEM_data!$G155:$L155)</f>
+        <v>7449.95</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -27993,8 +27993,8 @@
         <v>1</v>
       </c>
       <c r="G156">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D156:$E156,raw_OpenNEM_data!$G156:$L156)</f>
+        <v>7499.2999999999993</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -28022,8 +28022,8 @@
         <v>1</v>
       </c>
       <c r="G157">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D157:$E157,raw_OpenNEM_data!$G157:$L157)</f>
+        <v>7226.3499999999995</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -28051,8 +28051,8 @@
         <v>1</v>
       </c>
       <c r="G158">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D158:$E158,raw_OpenNEM_data!$G158:$L158)</f>
+        <v>7216.6900000000005</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -28080,8 +28080,8 @@
         <v>1</v>
       </c>
       <c r="G159">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D159:$E159,raw_OpenNEM_data!$G159:$L159)</f>
+        <v>7113.21</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -28109,8 +28109,8 @@
         <v>1</v>
       </c>
       <c r="G160">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D160:$E160,raw_OpenNEM_data!$G160:$L160)</f>
+        <v>6875.5300000000007</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -28138,8 +28138,8 @@
         <v>1</v>
       </c>
       <c r="G161">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D161:$E161,raw_OpenNEM_data!$G161:$L161)</f>
+        <v>6563.1200000000017</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -28167,8 +28167,8 @@
         <v>1</v>
       </c>
       <c r="G162">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D162:$E162,raw_OpenNEM_data!$G162:$L162)</f>
+        <v>6272.39</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
@@ -28196,8 +28196,8 @@
         <v>1</v>
       </c>
       <c r="G163">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D163:$E163,raw_OpenNEM_data!$G163:$L163)</f>
+        <v>5995.1500000000005</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -28225,8 +28225,8 @@
         <v>1</v>
       </c>
       <c r="G164">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D164:$E164,raw_OpenNEM_data!$G164:$L164)</f>
+        <v>5911.4500000000007</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -28254,8 +28254,8 @@
         <v>1</v>
       </c>
       <c r="G165">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D165:$E165,raw_OpenNEM_data!$G165:$L165)</f>
+        <v>5840.87</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -28283,8 +28283,8 @@
         <v>1</v>
       </c>
       <c r="G166">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D166:$E166,raw_OpenNEM_data!$G166:$L166)</f>
+        <v>5804.3300000000008</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -28312,8 +28312,8 @@
         <v>1</v>
       </c>
       <c r="G167">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D167:$E167,raw_OpenNEM_data!$G167:$L167)</f>
+        <v>5815.2000000000007</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -28341,8 +28341,8 @@
         <v>1</v>
       </c>
       <c r="G168">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D168:$E168,raw_OpenNEM_data!$G168:$L168)</f>
+        <v>5938.4000000000015</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -28370,8 +28370,8 @@
         <v>1</v>
       </c>
       <c r="G169">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D169:$E169,raw_OpenNEM_data!$G169:$L169)</f>
+        <v>6064</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -28399,8 +28399,8 @@
         <v>1</v>
       </c>
       <c r="G170">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D170:$E170,raw_OpenNEM_data!$G170:$L170)</f>
+        <v>6301.5500000000011</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -28428,8 +28428,8 @@
         <v>1</v>
       </c>
       <c r="G171">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D171:$E171,raw_OpenNEM_data!$G171:$L171)</f>
+        <v>6523.4699999999993</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -28457,8 +28457,8 @@
         <v>1</v>
       </c>
       <c r="G172">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D172:$E172,raw_OpenNEM_data!$G172:$L172)</f>
+        <v>6851.81</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -28486,8 +28486,8 @@
         <v>1</v>
       </c>
       <c r="G173">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D173:$E173,raw_OpenNEM_data!$G173:$L173)</f>
+        <v>7117.73</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -28515,8 +28515,8 @@
         <v>1</v>
       </c>
       <c r="G174">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D174:$E174,raw_OpenNEM_data!$G174:$L174)</f>
+        <v>7375.869999999999</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -28544,8 +28544,8 @@
         <v>1</v>
       </c>
       <c r="G175">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D175:$E175,raw_OpenNEM_data!$G175:$L175)</f>
+        <v>7627.5599999999995</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -28573,8 +28573,8 @@
         <v>1</v>
       </c>
       <c r="G176">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D176:$E176,raw_OpenNEM_data!$G176:$L176)</f>
+        <v>7914.36</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -28602,8 +28602,8 @@
         <v>1</v>
       </c>
       <c r="G177">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D177:$E177,raw_OpenNEM_data!$G177:$L177)</f>
+        <v>8008.4</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
@@ -28631,8 +28631,8 @@
         <v>1</v>
       </c>
       <c r="G178">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D178:$E178,raw_OpenNEM_data!$G178:$L178)</f>
+        <v>8221.02</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
@@ -28660,8 +28660,8 @@
         <v>1</v>
       </c>
       <c r="G179">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D179:$E179,raw_OpenNEM_data!$G179:$L179)</f>
+        <v>8316.1</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -28689,8 +28689,8 @@
         <v>1</v>
       </c>
       <c r="G180">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D180:$E180,raw_OpenNEM_data!$G180:$L180)</f>
+        <v>8321.69</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -28718,8 +28718,8 @@
         <v>1</v>
       </c>
       <c r="G181">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D181:$E181,raw_OpenNEM_data!$G181:$L181)</f>
+        <v>8348.0299999999988</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
@@ -28747,8 +28747,8 @@
         <v>1</v>
       </c>
       <c r="G182">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D182:$E182,raw_OpenNEM_data!$G182:$L182)</f>
+        <v>8272.7099999999991</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
@@ -28776,8 +28776,8 @@
         <v>1</v>
       </c>
       <c r="G183">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D183:$E183,raw_OpenNEM_data!$G183:$L183)</f>
+        <v>8193.0499999999993</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
@@ -28805,8 +28805,8 @@
         <v>1</v>
       </c>
       <c r="G184">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D184:$E184,raw_OpenNEM_data!$G184:$L184)</f>
+        <v>8150.57</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
@@ -28834,8 +28834,8 @@
         <v>1</v>
       </c>
       <c r="G185">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D185:$E185,raw_OpenNEM_data!$G185:$L185)</f>
+        <v>8320.99</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
@@ -28863,8 +28863,8 @@
         <v>1</v>
       </c>
       <c r="G186">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D186:$E186,raw_OpenNEM_data!$G186:$L186)</f>
+        <v>8315.2699999999986</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
@@ -28892,8 +28892,8 @@
         <v>1</v>
       </c>
       <c r="G187">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D187:$E187,raw_OpenNEM_data!$G187:$L187)</f>
+        <v>8210.9199999999983</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
@@ -28921,8 +28921,8 @@
         <v>1</v>
       </c>
       <c r="G188">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D188:$E188,raw_OpenNEM_data!$G188:$L188)</f>
+        <v>8254.9399999999987</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
@@ -28950,8 +28950,8 @@
         <v>1</v>
       </c>
       <c r="G189">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D189:$E189,raw_OpenNEM_data!$G189:$L189)</f>
+        <v>8235.0799999999981</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -28979,8 +28979,8 @@
         <v>1</v>
       </c>
       <c r="G190">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D190:$E190,raw_OpenNEM_data!$G190:$L190)</f>
+        <v>8311.24</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -29008,8 +29008,8 @@
         <v>1</v>
       </c>
       <c r="G191">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D191:$E191,raw_OpenNEM_data!$G191:$L191)</f>
+        <v>8303.52</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
@@ -29037,8 +29037,8 @@
         <v>1</v>
       </c>
       <c r="G192">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D192:$E192,raw_OpenNEM_data!$G192:$L192)</f>
+        <v>8360.26</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -29066,8 +29066,8 @@
         <v>1</v>
       </c>
       <c r="G193">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D193:$E193,raw_OpenNEM_data!$G193:$L193)</f>
+        <v>8176.18</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
@@ -29095,8 +29095,8 @@
         <v>1</v>
       </c>
       <c r="G194">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D194:$E194,raw_OpenNEM_data!$G194:$L194)</f>
+        <v>8033.5</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -29124,8 +29124,8 @@
         <v>1</v>
       </c>
       <c r="G195">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D195:$E195,raw_OpenNEM_data!$G195:$L195)</f>
+        <v>7928.76</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
@@ -29153,8 +29153,8 @@
         <v>1</v>
       </c>
       <c r="G196">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D196:$E196,raw_OpenNEM_data!$G196:$L196)</f>
+        <v>7814.4799999999987</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
@@ -29182,8 +29182,8 @@
         <v>1</v>
       </c>
       <c r="G197">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D197:$E197,raw_OpenNEM_data!$G197:$L197)</f>
+        <v>7661.45</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
@@ -29211,8 +29211,8 @@
         <v>1</v>
       </c>
       <c r="G198">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D198:$E198,raw_OpenNEM_data!$G198:$L198)</f>
+        <v>7683.75</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -29240,8 +29240,8 @@
         <v>1</v>
       </c>
       <c r="G199">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D199:$E199,raw_OpenNEM_data!$G199:$L199)</f>
+        <v>7659.0000000000009</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -29269,8 +29269,8 @@
         <v>1</v>
       </c>
       <c r="G200">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D200:$E200,raw_OpenNEM_data!$G200:$L200)</f>
+        <v>7532.9500000000007</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
@@ -29298,8 +29298,8 @@
         <v>1</v>
       </c>
       <c r="G201">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D201:$E201,raw_OpenNEM_data!$G201:$L201)</f>
+        <v>7400.81</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
@@ -29327,8 +29327,8 @@
         <v>1</v>
       </c>
       <c r="G202">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D202:$E202,raw_OpenNEM_data!$G202:$L202)</f>
+        <v>7411.36</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
@@ -29356,8 +29356,8 @@
         <v>1</v>
       </c>
       <c r="G203">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D203:$E203,raw_OpenNEM_data!$G203:$L203)</f>
+        <v>7288.5500000000011</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
@@ -29385,8 +29385,8 @@
         <v>1</v>
       </c>
       <c r="G204">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D204:$E204,raw_OpenNEM_data!$G204:$L204)</f>
+        <v>7325.09</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
@@ -29414,8 +29414,8 @@
         <v>1</v>
       </c>
       <c r="G205">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D205:$E205,raw_OpenNEM_data!$G205:$L205)</f>
+        <v>7136.4000000000005</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
@@ -29443,8 +29443,8 @@
         <v>1</v>
       </c>
       <c r="G206">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D206:$E206,raw_OpenNEM_data!$G206:$L206)</f>
+        <v>7057.72</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -29472,8 +29472,8 @@
         <v>1</v>
       </c>
       <c r="G207">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D207:$E207,raw_OpenNEM_data!$G207:$L207)</f>
+        <v>6929.6600000000008</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
@@ -29501,8 +29501,8 @@
         <v>1</v>
       </c>
       <c r="G208">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D208:$E208,raw_OpenNEM_data!$G208:$L208)</f>
+        <v>6765.1100000000006</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
@@ -29530,8 +29530,8 @@
         <v>1</v>
       </c>
       <c r="G209">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D209:$E209,raw_OpenNEM_data!$G209:$L209)</f>
+        <v>6544.22</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
@@ -29559,8 +29559,8 @@
         <v>1</v>
       </c>
       <c r="G210">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D210:$E210,raw_OpenNEM_data!$G210:$L210)</f>
+        <v>6205.7</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
@@ -29588,8 +29588,8 @@
         <v>1</v>
       </c>
       <c r="G211">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D211:$E211,raw_OpenNEM_data!$G211:$L211)</f>
+        <v>6021.4199999999992</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
@@ -29617,8 +29617,8 @@
         <v>1</v>
       </c>
       <c r="G212">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D212:$E212,raw_OpenNEM_data!$G212:$L212)</f>
+        <v>5868.2300000000014</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
@@ -29646,8 +29646,8 @@
         <v>1</v>
       </c>
       <c r="G213">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D213:$E213,raw_OpenNEM_data!$G213:$L213)</f>
+        <v>5836.1400000000012</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -29675,8 +29675,8 @@
         <v>1</v>
       </c>
       <c r="G214">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D214:$E214,raw_OpenNEM_data!$G214:$L214)</f>
+        <v>5776.0300000000016</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -29704,8 +29704,8 @@
         <v>1</v>
       </c>
       <c r="G215">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D215:$E215,raw_OpenNEM_data!$G215:$L215)</f>
+        <v>5811.87</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
@@ -29733,8 +29733,8 @@
         <v>1</v>
       </c>
       <c r="G216">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D216:$E216,raw_OpenNEM_data!$G216:$L216)</f>
+        <v>5902.32</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
@@ -29762,8 +29762,8 @@
         <v>1</v>
       </c>
       <c r="G217">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D217:$E217,raw_OpenNEM_data!$G217:$L217)</f>
+        <v>6013.37</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
@@ -29791,8 +29791,8 @@
         <v>1</v>
       </c>
       <c r="G218">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D218:$E218,raw_OpenNEM_data!$G218:$L218)</f>
+        <v>6264.8499999999995</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
@@ -29820,8 +29820,8 @@
         <v>1</v>
       </c>
       <c r="G219">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D219:$E219,raw_OpenNEM_data!$G219:$L219)</f>
+        <v>6451.5499999999993</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -29849,8 +29849,8 @@
         <v>1</v>
       </c>
       <c r="G220">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D220:$E220,raw_OpenNEM_data!$G220:$L220)</f>
+        <v>6829.6000000000013</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
@@ -29878,8 +29878,8 @@
         <v>1</v>
       </c>
       <c r="G221">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D221:$E221,raw_OpenNEM_data!$G221:$L221)</f>
+        <v>7044.39</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
@@ -29907,8 +29907,8 @@
         <v>1</v>
       </c>
       <c r="G222">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D222:$E222,raw_OpenNEM_data!$G222:$L222)</f>
+        <v>7379.03</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
@@ -29936,8 +29936,8 @@
         <v>1</v>
       </c>
       <c r="G223">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D223:$E223,raw_OpenNEM_data!$G223:$L223)</f>
+        <v>7710.76</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
@@ -29965,8 +29965,8 @@
         <v>1</v>
       </c>
       <c r="G224">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D224:$E224,raw_OpenNEM_data!$G224:$L224)</f>
+        <v>7965.47</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -29994,8 +29994,8 @@
         <v>1</v>
       </c>
       <c r="G225">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D225:$E225,raw_OpenNEM_data!$G225:$L225)</f>
+        <v>8022.8799999999992</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
@@ -30023,8 +30023,8 @@
         <v>1</v>
       </c>
       <c r="G226">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D226:$E226,raw_OpenNEM_data!$G226:$L226)</f>
+        <v>8240.52</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
@@ -30052,8 +30052,8 @@
         <v>1</v>
       </c>
       <c r="G227">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D227:$E227,raw_OpenNEM_data!$G227:$L227)</f>
+        <v>8283.369999999999</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -30081,8 +30081,8 @@
         <v>1</v>
       </c>
       <c r="G228">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D228:$E228,raw_OpenNEM_data!$G228:$L228)</f>
+        <v>8373.66</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -30110,8 +30110,8 @@
         <v>1</v>
       </c>
       <c r="G229">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D229:$E229,raw_OpenNEM_data!$G229:$L229)</f>
+        <v>8328.68</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -30139,8 +30139,8 @@
         <v>1</v>
       </c>
       <c r="G230">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D230:$E230,raw_OpenNEM_data!$G230:$L230)</f>
+        <v>8328.32</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -30168,8 +30168,8 @@
         <v>1</v>
       </c>
       <c r="G231">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D231:$E231,raw_OpenNEM_data!$G231:$L231)</f>
+        <v>8276.82</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -30197,8 +30197,8 @@
         <v>1</v>
       </c>
       <c r="G232">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D232:$E232,raw_OpenNEM_data!$G232:$L232)</f>
+        <v>8201.1</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -30226,8 +30226,8 @@
         <v>1</v>
       </c>
       <c r="G233">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D233:$E233,raw_OpenNEM_data!$G233:$L233)</f>
+        <v>8110.5599999999995</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -30255,8 +30255,8 @@
         <v>1</v>
       </c>
       <c r="G234">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D234:$E234,raw_OpenNEM_data!$G234:$L234)</f>
+        <v>8153.57</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -30284,8 +30284,8 @@
         <v>1</v>
       </c>
       <c r="G235">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D235:$E235,raw_OpenNEM_data!$G235:$L235)</f>
+        <v>8085.6900000000005</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -30313,8 +30313,8 @@
         <v>1</v>
       </c>
       <c r="G236">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D236:$E236,raw_OpenNEM_data!$G236:$L236)</f>
+        <v>7977.1</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -30342,8 +30342,8 @@
         <v>1</v>
       </c>
       <c r="G237">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D237:$E237,raw_OpenNEM_data!$G237:$L237)</f>
+        <v>7973.0099999999993</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -30371,8 +30371,8 @@
         <v>1</v>
       </c>
       <c r="G238">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D238:$E238,raw_OpenNEM_data!$G238:$L238)</f>
+        <v>7894.0400000000009</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
@@ -30400,8 +30400,8 @@
         <v>1</v>
       </c>
       <c r="G239">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D239:$E239,raw_OpenNEM_data!$G239:$L239)</f>
+        <v>7968.36</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -30429,8 +30429,8 @@
         <v>1</v>
       </c>
       <c r="G240">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D240:$E240,raw_OpenNEM_data!$G240:$L240)</f>
+        <v>8018.9800000000014</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
@@ -30458,8 +30458,8 @@
         <v>1</v>
       </c>
       <c r="G241">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D241:$E241,raw_OpenNEM_data!$G241:$L241)</f>
+        <v>7976.85</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -30487,8 +30487,8 @@
         <v>1</v>
       </c>
       <c r="G242">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D242:$E242,raw_OpenNEM_data!$G242:$L242)</f>
+        <v>7755.5000000000009</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -30516,8 +30516,8 @@
         <v>1</v>
       </c>
       <c r="G243">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D243:$E243,raw_OpenNEM_data!$G243:$L243)</f>
+        <v>7642.2400000000007</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
@@ -30545,8 +30545,8 @@
         <v>1</v>
       </c>
       <c r="G244">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D244:$E244,raw_OpenNEM_data!$G244:$L244)</f>
+        <v>7472.7400000000007</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
@@ -30574,8 +30574,8 @@
         <v>1</v>
       </c>
       <c r="G245">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D245:$E245,raw_OpenNEM_data!$G245:$L245)</f>
+        <v>7414.52</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -30603,8 +30603,8 @@
         <v>1</v>
       </c>
       <c r="G246">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D246:$E246,raw_OpenNEM_data!$G246:$L246)</f>
+        <v>7343.170000000001</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -30632,8 +30632,8 @@
         <v>1</v>
       </c>
       <c r="G247">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D247:$E247,raw_OpenNEM_data!$G247:$L247)</f>
+        <v>7293.57</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -30661,8 +30661,8 @@
         <v>1</v>
       </c>
       <c r="G248">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D248:$E248,raw_OpenNEM_data!$G248:$L248)</f>
+        <v>7159.4099999999989</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
@@ -30690,8 +30690,8 @@
         <v>1</v>
       </c>
       <c r="G249">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D249:$E249,raw_OpenNEM_data!$G249:$L249)</f>
+        <v>7148.43</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
@@ -30719,8 +30719,8 @@
         <v>1</v>
       </c>
       <c r="G250">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D250:$E250,raw_OpenNEM_data!$G250:$L250)</f>
+        <v>7182.3</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
@@ -30748,8 +30748,8 @@
         <v>1</v>
       </c>
       <c r="G251">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D251:$E251,raw_OpenNEM_data!$G251:$L251)</f>
+        <v>7230.9800000000014</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -30777,8 +30777,8 @@
         <v>1</v>
       </c>
       <c r="G252">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D252:$E252,raw_OpenNEM_data!$G252:$L252)</f>
+        <v>7248.4800000000005</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
@@ -30806,8 +30806,8 @@
         <v>1</v>
       </c>
       <c r="G253">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D253:$E253,raw_OpenNEM_data!$G253:$L253)</f>
+        <v>7190.65</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -30835,8 +30835,8 @@
         <v>1</v>
       </c>
       <c r="G254">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D254:$E254,raw_OpenNEM_data!$G254:$L254)</f>
+        <v>7167.04</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -30864,8 +30864,8 @@
         <v>1</v>
       </c>
       <c r="G255">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D255:$E255,raw_OpenNEM_data!$G255:$L255)</f>
+        <v>7024.97</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -30893,8 +30893,8 @@
         <v>1</v>
       </c>
       <c r="G256">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D256:$E256,raw_OpenNEM_data!$G256:$L256)</f>
+        <v>6817.8600000000006</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -30922,8 +30922,8 @@
         <v>1</v>
       </c>
       <c r="G257">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D257:$E257,raw_OpenNEM_data!$G257:$L257)</f>
+        <v>6582.89</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
@@ -30951,8 +30951,8 @@
         <v>1</v>
       </c>
       <c r="G258">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D258:$E258,raw_OpenNEM_data!$G258:$L258)</f>
+        <v>6279.6800000000012</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -30980,8 +30980,8 @@
         <v>1</v>
       </c>
       <c r="G259">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D259:$E259,raw_OpenNEM_data!$G259:$L259)</f>
+        <v>6031</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -31009,8 +31009,8 @@
         <v>1</v>
       </c>
       <c r="G260">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D260:$E260,raw_OpenNEM_data!$G260:$L260)</f>
+        <v>5844.16</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -31038,8 +31038,8 @@
         <v>1</v>
       </c>
       <c r="G261">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D261:$E261,raw_OpenNEM_data!$G261:$L261)</f>
+        <v>5782.6699999999983</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -31067,8 +31067,8 @@
         <v>1</v>
       </c>
       <c r="G262">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D262:$E262,raw_OpenNEM_data!$G262:$L262)</f>
+        <v>5674.4000000000015</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
@@ -31096,8 +31096,8 @@
         <v>1</v>
       </c>
       <c r="G263">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D263:$E263,raw_OpenNEM_data!$G263:$L263)</f>
+        <v>5689.2400000000016</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
@@ -31125,8 +31125,8 @@
         <v>1</v>
       </c>
       <c r="G264">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D264:$E264,raw_OpenNEM_data!$G264:$L264)</f>
+        <v>5727.38</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
@@ -31154,8 +31154,8 @@
         <v>1</v>
       </c>
       <c r="G265">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D265:$E265,raw_OpenNEM_data!$G265:$L265)</f>
+        <v>5755.3899999999994</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
@@ -31183,8 +31183,8 @@
         <v>1</v>
       </c>
       <c r="G266">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D266:$E266,raw_OpenNEM_data!$G266:$L266)</f>
+        <v>5854.61</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
@@ -31212,8 +31212,8 @@
         <v>1</v>
       </c>
       <c r="G267">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D267:$E267,raw_OpenNEM_data!$G267:$L267)</f>
+        <v>5961.8399999999992</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
@@ -31241,8 +31241,8 @@
         <v>1</v>
       </c>
       <c r="G268">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D268:$E268,raw_OpenNEM_data!$G268:$L268)</f>
+        <v>6127.23</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.3">
@@ -31270,8 +31270,8 @@
         <v>1</v>
       </c>
       <c r="G269">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D269:$E269,raw_OpenNEM_data!$G269:$L269)</f>
+        <v>6327.52</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
@@ -31299,8 +31299,8 @@
         <v>1</v>
       </c>
       <c r="G270">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D270:$E270,raw_OpenNEM_data!$G270:$L270)</f>
+        <v>6530.9399999999987</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
@@ -31328,8 +31328,8 @@
         <v>1</v>
       </c>
       <c r="G271">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D271:$E271,raw_OpenNEM_data!$G271:$L271)</f>
+        <v>6794.3900000000012</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
@@ -31357,8 +31357,8 @@
         <v>1</v>
       </c>
       <c r="G272">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D272:$E272,raw_OpenNEM_data!$G272:$L272)</f>
+        <v>7019.11</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.3">
@@ -31386,8 +31386,8 @@
         <v>1</v>
       </c>
       <c r="G273">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D273:$E273,raw_OpenNEM_data!$G273:$L273)</f>
+        <v>7191.6900000000005</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
@@ -31415,8 +31415,8 @@
         <v>1</v>
       </c>
       <c r="G274">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D274:$E274,raw_OpenNEM_data!$G274:$L274)</f>
+        <v>7381.96</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
@@ -31444,8 +31444,8 @@
         <v>1</v>
       </c>
       <c r="G275">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D275:$E275,raw_OpenNEM_data!$G275:$L275)</f>
+        <v>7429.07</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
@@ -31473,8 +31473,8 @@
         <v>1</v>
       </c>
       <c r="G276">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D276:$E276,raw_OpenNEM_data!$G276:$L276)</f>
+        <v>7527.1100000000006</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
@@ -31502,8 +31502,8 @@
         <v>1</v>
       </c>
       <c r="G277">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D277:$E277,raw_OpenNEM_data!$G277:$L277)</f>
+        <v>7586.61</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
@@ -31531,8 +31531,8 @@
         <v>1</v>
       </c>
       <c r="G278">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D278:$E278,raw_OpenNEM_data!$G278:$L278)</f>
+        <v>7602.8099999999995</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.3">
@@ -31560,8 +31560,8 @@
         <v>1</v>
       </c>
       <c r="G279">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D279:$E279,raw_OpenNEM_data!$G279:$L279)</f>
+        <v>7583.05</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.3">
@@ -31589,8 +31589,8 @@
         <v>1</v>
       </c>
       <c r="G280">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D280:$E280,raw_OpenNEM_data!$G280:$L280)</f>
+        <v>7501.51</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
@@ -31618,8 +31618,8 @@
         <v>1</v>
       </c>
       <c r="G281">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D281:$E281,raw_OpenNEM_data!$G281:$L281)</f>
+        <v>7467.59</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.3">
@@ -31647,8 +31647,8 @@
         <v>1</v>
       </c>
       <c r="G282">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D282:$E282,raw_OpenNEM_data!$G282:$L282)</f>
+        <v>7383.48</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.3">
@@ -31676,8 +31676,8 @@
         <v>1</v>
       </c>
       <c r="G283">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D283:$E283,raw_OpenNEM_data!$G283:$L283)</f>
+        <v>7300.5599999999995</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.3">
@@ -31705,8 +31705,8 @@
         <v>1</v>
       </c>
       <c r="G284">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D284:$E284,raw_OpenNEM_data!$G284:$L284)</f>
+        <v>7294.4</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.3">
@@ -31734,8 +31734,8 @@
         <v>1</v>
       </c>
       <c r="G285">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D285:$E285,raw_OpenNEM_data!$G285:$L285)</f>
+        <v>7268.19</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.3">
@@ -31763,8 +31763,8 @@
         <v>1</v>
       </c>
       <c r="G286">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D286:$E286,raw_OpenNEM_data!$G286:$L286)</f>
+        <v>7235.27</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.3">
@@ -31792,8 +31792,8 @@
         <v>1</v>
       </c>
       <c r="G287">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D287:$E287,raw_OpenNEM_data!$G287:$L287)</f>
+        <v>7335.0899999999992</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.3">
@@ -31821,8 +31821,8 @@
         <v>1</v>
       </c>
       <c r="G288">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D288:$E288,raw_OpenNEM_data!$G288:$L288)</f>
+        <v>7394.1399999999994</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.3">
@@ -31850,8 +31850,8 @@
         <v>1</v>
       </c>
       <c r="G289">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D289:$E289,raw_OpenNEM_data!$G289:$L289)</f>
+        <v>7402.85</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.3">
@@ -31879,8 +31879,8 @@
         <v>1</v>
       </c>
       <c r="G290">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D290:$E290,raw_OpenNEM_data!$G290:$L290)</f>
+        <v>7398.3600000000006</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.3">
@@ -31908,8 +31908,8 @@
         <v>1</v>
       </c>
       <c r="G291">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D291:$E291,raw_OpenNEM_data!$G291:$L291)</f>
+        <v>7347.46</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.3">
@@ -31937,8 +31937,8 @@
         <v>1</v>
       </c>
       <c r="G292">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D292:$E292,raw_OpenNEM_data!$G292:$L292)</f>
+        <v>7242.18</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.3">
@@ -31966,8 +31966,8 @@
         <v>1</v>
       </c>
       <c r="G293">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D293:$E293,raw_OpenNEM_data!$G293:$L293)</f>
+        <v>7193.69</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.3">
@@ -31995,8 +31995,8 @@
         <v>1</v>
       </c>
       <c r="G294">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D294:$E294,raw_OpenNEM_data!$G294:$L294)</f>
+        <v>7266.7699999999986</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.3">
@@ -32024,8 +32024,8 @@
         <v>1</v>
       </c>
       <c r="G295">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D295:$E295,raw_OpenNEM_data!$G295:$L295)</f>
+        <v>7188.18</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.3">
@@ -32053,8 +32053,8 @@
         <v>1</v>
       </c>
       <c r="G296">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D296:$E296,raw_OpenNEM_data!$G296:$L296)</f>
+        <v>7108.7800000000007</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.3">
@@ -32082,8 +32082,8 @@
         <v>1</v>
       </c>
       <c r="G297">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D297:$E297,raw_OpenNEM_data!$G297:$L297)</f>
+        <v>7008.4500000000007</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.3">
@@ -32111,8 +32111,8 @@
         <v>1</v>
       </c>
       <c r="G298">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D298:$E298,raw_OpenNEM_data!$G298:$L298)</f>
+        <v>7052.3000000000011</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.3">
@@ -32140,8 +32140,8 @@
         <v>1</v>
       </c>
       <c r="G299">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D299:$E299,raw_OpenNEM_data!$G299:$L299)</f>
+        <v>7027.43</v>
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.3">
@@ -32169,8 +32169,8 @@
         <v>1</v>
       </c>
       <c r="G300">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D300:$E300,raw_OpenNEM_data!$G300:$L300)</f>
+        <v>7003.14</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.3">
@@ -32198,8 +32198,8 @@
         <v>1</v>
       </c>
       <c r="G301">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D301:$E301,raw_OpenNEM_data!$G301:$L301)</f>
+        <v>6938.7900000000018</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.3">
@@ -32227,8 +32227,8 @@
         <v>1</v>
       </c>
       <c r="G302">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D302:$E302,raw_OpenNEM_data!$G302:$L302)</f>
+        <v>6821.1600000000008</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.3">
@@ -32256,8 +32256,8 @@
         <v>1</v>
       </c>
       <c r="G303">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D303:$E303,raw_OpenNEM_data!$G303:$L303)</f>
+        <v>6675.88</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.3">
@@ -32285,8 +32285,8 @@
         <v>1</v>
       </c>
       <c r="G304">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D304:$E304,raw_OpenNEM_data!$G304:$L304)</f>
+        <v>6477.3</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.3">
@@ -32314,8 +32314,8 @@
         <v>1</v>
       </c>
       <c r="G305">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D305:$E305,raw_OpenNEM_data!$G305:$L305)</f>
+        <v>6253.6100000000006</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.3">
@@ -32343,8 +32343,8 @@
         <v>1</v>
       </c>
       <c r="G306">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D306:$E306,raw_OpenNEM_data!$G306:$L306)</f>
+        <v>5997.1000000000013</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.3">
@@ -32372,8 +32372,8 @@
         <v>1</v>
       </c>
       <c r="G307">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D307:$E307,raw_OpenNEM_data!$G307:$L307)</f>
+        <v>5826.82</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.3">
@@ -32401,8 +32401,8 @@
         <v>1</v>
       </c>
       <c r="G308">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D308:$E308,raw_OpenNEM_data!$G308:$L308)</f>
+        <v>5714.4100000000008</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.3">
@@ -32430,8 +32430,8 @@
         <v>1</v>
       </c>
       <c r="G309">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D309:$E309,raw_OpenNEM_data!$G309:$L309)</f>
+        <v>5605.26</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.3">
@@ -32459,8 +32459,8 @@
         <v>1</v>
       </c>
       <c r="G310">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D310:$E310,raw_OpenNEM_data!$G310:$L310)</f>
+        <v>5591.7900000000009</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.3">
@@ -32488,8 +32488,8 @@
         <v>1</v>
       </c>
       <c r="G311">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D311:$E311,raw_OpenNEM_data!$G311:$L311)</f>
+        <v>5629.4400000000014</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.3">
@@ -32517,8 +32517,8 @@
         <v>1</v>
       </c>
       <c r="G312">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D312:$E312,raw_OpenNEM_data!$G312:$L312)</f>
+        <v>5664.04</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.3">
@@ -32546,8 +32546,8 @@
         <v>1</v>
       </c>
       <c r="G313">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D313:$E313,raw_OpenNEM_data!$G313:$L313)</f>
+        <v>5747.25</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.3">
@@ -32575,8 +32575,8 @@
         <v>1</v>
       </c>
       <c r="G314">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D314:$E314,raw_OpenNEM_data!$G314:$L314)</f>
+        <v>5874.3300000000008</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.3">
@@ -32604,8 +32604,8 @@
         <v>1</v>
       </c>
       <c r="G315">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D315:$E315,raw_OpenNEM_data!$G315:$L315)</f>
+        <v>6051.3499999999995</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.3">
@@ -32633,8 +32633,8 @@
         <v>1</v>
       </c>
       <c r="G316">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D316:$E316,raw_OpenNEM_data!$G316:$L316)</f>
+        <v>6323.47</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.3">
@@ -32662,8 +32662,8 @@
         <v>1</v>
       </c>
       <c r="G317">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D317:$E317,raw_OpenNEM_data!$G317:$L317)</f>
+        <v>6596.16</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.3">
@@ -32691,8 +32691,8 @@
         <v>1</v>
       </c>
       <c r="G318">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D318:$E318,raw_OpenNEM_data!$G318:$L318)</f>
+        <v>6926.119999999999</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.3">
@@ -32720,8 +32720,8 @@
         <v>1</v>
       </c>
       <c r="G319">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D319:$E319,raw_OpenNEM_data!$G319:$L319)</f>
+        <v>7208.77</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.3">
@@ -32749,8 +32749,8 @@
         <v>1</v>
       </c>
       <c r="G320">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D320:$E320,raw_OpenNEM_data!$G320:$L320)</f>
+        <v>7434.86</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.3">
@@ -32778,8 +32778,8 @@
         <v>1</v>
       </c>
       <c r="G321">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D321:$E321,raw_OpenNEM_data!$G321:$L321)</f>
+        <v>7530.58</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.3">
@@ -32807,8 +32807,8 @@
         <v>1</v>
       </c>
       <c r="G322">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D322:$E322,raw_OpenNEM_data!$G322:$L322)</f>
+        <v>7603.7500000000009</v>
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.3">
@@ -32836,8 +32836,8 @@
         <v>1</v>
       </c>
       <c r="G323">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D323:$E323,raw_OpenNEM_data!$G323:$L323)</f>
+        <v>7675.0700000000015</v>
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.3">
@@ -32865,8 +32865,8 @@
         <v>1</v>
       </c>
       <c r="G324">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D324:$E324,raw_OpenNEM_data!$G324:$L324)</f>
+        <v>7767.11</v>
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.3">
@@ -32894,8 +32894,8 @@
         <v>1</v>
       </c>
       <c r="G325">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D325:$E325,raw_OpenNEM_data!$G325:$L325)</f>
+        <v>7698.27</v>
       </c>
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.3">
@@ -32923,8 +32923,8 @@
         <v>1</v>
       </c>
       <c r="G326">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D326:$E326,raw_OpenNEM_data!$G326:$L326)</f>
+        <v>7708.8499999999985</v>
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.3">
@@ -32952,8 +32952,8 @@
         <v>1</v>
       </c>
       <c r="G327">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D327:$E327,raw_OpenNEM_data!$G327:$L327)</f>
+        <v>7715.130000000001</v>
       </c>
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.3">
@@ -32981,8 +32981,8 @@
         <v>1</v>
       </c>
       <c r="G328">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D328:$E328,raw_OpenNEM_data!$G328:$L328)</f>
+        <v>7630.59</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.3">
@@ -33010,8 +33010,8 @@
         <v>1</v>
       </c>
       <c r="G329">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D329:$E329,raw_OpenNEM_data!$G329:$L329)</f>
+        <v>7581.8600000000006</v>
       </c>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.3">
@@ -33039,8 +33039,8 @@
         <v>1</v>
       </c>
       <c r="G330">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D330:$E330,raw_OpenNEM_data!$G330:$L330)</f>
+        <v>7560.74</v>
       </c>
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.3">
@@ -33068,8 +33068,8 @@
         <v>1</v>
       </c>
       <c r="G331">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D331:$E331,raw_OpenNEM_data!$G331:$L331)</f>
+        <v>7652.2999999999993</v>
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.3">
@@ -33097,8 +33097,8 @@
         <v>1</v>
       </c>
       <c r="G332">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D332:$E332,raw_OpenNEM_data!$G332:$L332)</f>
+        <v>7618.58</v>
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.3">
@@ -33126,8 +33126,8 @@
         <v>1</v>
       </c>
       <c r="G333">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D333:$E333,raw_OpenNEM_data!$G333:$L333)</f>
+        <v>7584.16</v>
       </c>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.3">
@@ -33155,8 +33155,8 @@
         <v>1</v>
       </c>
       <c r="G334">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D334:$E334,raw_OpenNEM_data!$G334:$L334)</f>
+        <v>7508.45</v>
       </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.3">
@@ -33184,8 +33184,8 @@
         <v>1</v>
       </c>
       <c r="G335">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D335:$E335,raw_OpenNEM_data!$G335:$L335)</f>
+        <v>7627.1499999999987</v>
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.3">
@@ -33213,8 +33213,8 @@
         <v>1</v>
       </c>
       <c r="G336">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D336:$E336,raw_OpenNEM_data!$G336:$L336)</f>
+        <v>7647.5899999999992</v>
       </c>
     </row>
     <row r="337" spans="1:7" x14ac:dyDescent="0.3">
@@ -33242,8 +33242,8 @@
         <v>1</v>
       </c>
       <c r="G337">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D337:$E337,raw_OpenNEM_data!$G337:$L337)</f>
+        <v>7694.06</v>
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.3">
@@ -33271,8 +33271,8 @@
         <v>1</v>
       </c>
       <c r="G338">
-        <f>SUM(raw_OpenNEM_data!D$2:E$2,raw_OpenNEM_data!G$2:L$2)</f>
-        <v>7641.119999999999</v>
+        <f>SUM(raw_OpenNEM_data!$D338:$E338,raw_OpenNEM_data!$G338:$L338)</f>
+        <v>7619.1900000000014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>